<commit_message>
90% done task 2
</commit_message>
<xml_diff>
--- a/table_task2.xlsx
+++ b/table_task2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,28 +476,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NO2</t>
+          <t>DE_LU</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>39.26</v>
+        <v>37.67</v>
       </c>
       <c r="D2" t="n">
-        <v>38.81</v>
+        <v>38.06</v>
       </c>
       <c r="E2" t="n">
-        <v>8.23</v>
+        <v>15.52</v>
       </c>
       <c r="F2" t="n">
-        <v>5.86</v>
+        <v>-90.01000000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>109.45</v>
+        <v>121.46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -505,49 +505,49 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9.289999999999999</v>
+        <v>39.26</v>
       </c>
       <c r="D3" t="n">
-        <v>6.95</v>
+        <v>38.81</v>
       </c>
       <c r="E3" t="n">
-        <v>8.26</v>
+        <v>8.23</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.73</v>
+        <v>5.86</v>
       </c>
       <c r="G3" t="n">
-        <v>99.92</v>
+        <v>109.45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NO2</t>
+          <t>DE_LU</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>75.11</v>
+        <v>30.47</v>
       </c>
       <c r="D4" t="n">
-        <v>59.34</v>
+        <v>30.99</v>
       </c>
       <c r="E4" t="n">
-        <v>47.22</v>
+        <v>17.5</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.97</v>
+        <v>-83.94</v>
       </c>
       <c r="G4" t="n">
-        <v>600.16</v>
+        <v>200.04</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -555,43 +555,168 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>211.28</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>181.13</v>
+        <v>6.95</v>
       </c>
       <c r="E5" t="n">
-        <v>125.85</v>
+        <v>8.26</v>
       </c>
       <c r="F5" t="n">
-        <v>0.04</v>
+        <v>-1.73</v>
       </c>
       <c r="G5" t="n">
-        <v>844</v>
+        <v>99.92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DE_LU</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>96.84999999999999</v>
+      </c>
+      <c r="D6" t="n">
+        <v>75.48</v>
+      </c>
+      <c r="E6" t="n">
+        <v>73.68000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-69</v>
+      </c>
+      <c r="G6" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NO2</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>75.11</v>
+      </c>
+      <c r="D7" t="n">
+        <v>59.34</v>
+      </c>
+      <c r="E7" t="n">
+        <v>47.22</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-1.97</v>
+      </c>
+      <c r="G7" t="n">
+        <v>600.16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DE_LU</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>235.44</v>
+      </c>
+      <c r="D8" t="n">
+        <v>208.34</v>
+      </c>
+      <c r="E8" t="n">
+        <v>142.82</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-19.04</v>
+      </c>
+      <c r="G8" t="n">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>NO2</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>211.28</v>
+      </c>
+      <c r="D9" t="n">
+        <v>181.13</v>
+      </c>
+      <c r="E9" t="n">
+        <v>125.85</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G9" t="n">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>2023</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DE_LU</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>95.18000000000001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>98.02</v>
+      </c>
+      <c r="E10" t="n">
+        <v>47.58</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-500</v>
+      </c>
+      <c r="G10" t="n">
+        <v>524.27</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>NO2</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C11" t="n">
         <v>79.44</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D11" t="n">
         <v>80.45999999999999</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E11" t="n">
         <v>36.28</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F11" t="n">
         <v>-61.84</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G11" t="n">
         <v>261.85</v>
       </c>
     </row>

</xml_diff>